<commit_message>
removed list_index out of range error
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -676,7 +676,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -808,7 +812,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -878,7 +886,11 @@
           <t>Absent</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -948,7 +960,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
@@ -3452,7 +3468,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -3514,7 +3534,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -3642,7 +3666,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -3708,7 +3736,11 @@
           <t>Present</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>

</xml_diff>